<commit_message>
Añadida parte optativa práctica 5
</commit_message>
<xml_diff>
--- a/practicas/practica5/resultados.xlsx
+++ b/practicas/practica5/resultados.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45800" yWindow="460" windowWidth="31000" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hendrix" sheetId="1" r:id="rId1"/>
+    <sheet name="i7" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Threads</t>
   </si>
@@ -67,15 +68,39 @@
   <si>
     <t>Sun UltraSPARC T2 @ 1.20 GHz (4 cores, 8 threads/core)</t>
   </si>
+  <si>
+    <t>GNU Fortran (MacPorts gcc6 6.3.0_2) 6.3.0</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>sys</t>
+  </si>
+  <si>
+    <t>Intel(R) Core(TM) i7-4770 CPU @ 3.40GHz (4 cores, 2 threads/core)</t>
+  </si>
+  <si>
+    <t>Sistema operativo</t>
+  </si>
+  <si>
+    <t>Solaris 10</t>
+  </si>
+  <si>
+    <t>OS X 10.11.6 El Capitan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="168" formatCode="0.000000"/>
-    <numFmt numFmtId="169" formatCode="0.0000000"/>
-    <numFmt numFmtId="177" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -135,10 +160,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -149,27 +174,48 @@
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="14">
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.000000"/>
+      <numFmt numFmtId="166" formatCode="0.000000000000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="0.000000000000000"/>
+      <numFmt numFmtId="166" formatCode="0.000000000000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="177" formatCode="0.000000000000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -289,7 +335,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>hendrix!$B$18:$B$23</c:f>
+              <c:f>hendrix!$B$19:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -316,7 +362,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>hendrix!$H$18:$H$23</c:f>
+              <c:f>hendrix!$H$19:$H$24</c:f>
               <c:numCache>
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
@@ -375,7 +421,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>hendrix!$B$24:$B$29</c:f>
+              <c:f>hendrix!$B$25:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -402,7 +448,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>hendrix!$H$24:$H$29</c:f>
+              <c:f>hendrix!$H$25:$H$30</c:f>
               <c:numCache>
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
@@ -437,11 +483,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1460498064"/>
-        <c:axId val="1460922208"/>
+        <c:axId val="1511419104"/>
+        <c:axId val="1394587824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1460498064"/>
+        <c:axId val="1511419104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
@@ -555,14 +601,14 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1460922208"/>
+        <c:crossAx val="1394587824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4.0"/>
         <c:minorUnit val="2.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1460922208"/>
+        <c:axId val="1394587824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +678,453 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1460498064"/>
+        <c:crossAx val="1511419104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES_tradnl"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES_tradnl"/>
+              <a:t>Speedup con respecto a la versión secuencial</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>OpenMP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'i7'!$B$8:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'i7'!$H$8:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.988654781199352</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.963519313304721</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.711967545638946</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.80853277835588</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.80853277835588</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.80853277835588</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1455690480"/>
+        <c:axId val="1482911696"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1455690480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="32.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl"/>
+                  <a:t>Número de threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES_tradnl"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1482911696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4.0"/>
+        <c:minorUnit val="2.0"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1482911696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1455690480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -753,7 +1245,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1275,13 +2323,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>792480</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1304,9 +2352,46 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142240</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>81280</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A5:H29" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A5:H29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A6:H30" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A6:H30">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1321,15 +2406,47 @@
       <calculatedColumnFormula>"-xO3 -xopenmp"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Threads"/>
-    <tableColumn id="3" name="Resultado" dataDxfId="6"/>
-    <tableColumn id="4" name="Error" dataDxfId="5">
-      <calculatedColumnFormula>ABS($B$3-C6)</calculatedColumnFormula>
+    <tableColumn id="3" name="Resultado" dataDxfId="12"/>
+    <tableColumn id="4" name="Error" dataDxfId="11">
+      <calculatedColumnFormula>ABS($B$4-C7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="system_clock" dataDxfId="4"/>
-    <tableColumn id="6" name="dtime" dataDxfId="3"/>
-    <tableColumn id="7" name="etime" dataDxfId="2"/>
-    <tableColumn id="8" name="Speedup" dataDxfId="1">
-      <calculatedColumnFormula>$E$6/E6</calculatedColumnFormula>
+    <tableColumn id="5" name="system_clock" dataDxfId="10"/>
+    <tableColumn id="6" name="dtime" dataDxfId="9"/>
+    <tableColumn id="7" name="etime" dataDxfId="8"/>
+    <tableColumn id="8" name="Speedup" dataDxfId="7">
+      <calculatedColumnFormula>$E$7/E7</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A6:H13" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A6:H13">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Flags">
+      <calculatedColumnFormula>"-xO3 -xopenmp"</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="Threads"/>
+    <tableColumn id="3" name="Resultado" dataDxfId="5"/>
+    <tableColumn id="4" name="Error" dataDxfId="4">
+      <calculatedColumnFormula>ABS($B$4-C7)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="real" dataDxfId="3"/>
+    <tableColumn id="6" name="user" dataDxfId="2"/>
+    <tableColumn id="7" name="sys" dataDxfId="1"/>
+    <tableColumn id="8" name="Speedup" dataDxfId="0">
+      <calculatedColumnFormula>$E$7/E7</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1599,9 +2716,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1626,741 +2743,1039 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B4" s="4">
         <v>3.14159265358979</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="str">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
         <f>"-xO3"</f>
         <v>-xO3</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="2">
         <v>3.14159264413487</v>
       </c>
-      <c r="D6" s="2">
-        <f>ABS($B$3-C6)</f>
+      <c r="D7" s="2">
+        <f t="shared" ref="D7:D30" si="0">ABS($B$4-C7)</f>
         <v>9.4549199580740151E-9</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="1">
         <v>6.4832929999999998</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <v>6.4832210000000003</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G7" s="1">
         <v>6.4839969999999996</v>
       </c>
-      <c r="H6" s="1">
-        <f>$E$6/E6</f>
+      <c r="H7" s="1">
+        <f>$E$7/E7</f>
         <v>1</v>
       </c>
-      <c r="L6" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f t="shared" ref="A8:A12" si="1">"-xO3"</f>
+        <v>-xO3</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6.483314</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6.4832450000000001</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6.4840115999999997</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" ref="H8:H30" si="2">$E$7/E8</f>
+        <v>0.99999676091579082</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f t="shared" si="1"/>
+        <v>-xO3</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6.4811430000000003</v>
+      </c>
+      <c r="F9" s="1">
+        <v>6.4810720000000002</v>
+      </c>
+      <c r="G9" s="1">
+        <v>6.4818515000000003</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0003317316096867</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f t="shared" si="1"/>
+        <v>-xO3</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E10" s="1">
+        <v>6.4839989999999998</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6.4839260000000003</v>
+      </c>
+      <c r="G10" s="1">
+        <v>6.4846754000000004</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.99989111657790197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f t="shared" si="1"/>
+        <v>-xO3</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E11" s="1">
+        <v>6.4901900000000001</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6.4901090000000003</v>
+      </c>
+      <c r="G11" s="1">
+        <v>6.4908904999999999</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="2"/>
+        <v>0.99893731924643181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f t="shared" si="1"/>
+        <v>-xO3</v>
+      </c>
+      <c r="B12">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E12" s="1">
+        <v>6.4826360000000003</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6.4825660000000003</v>
+      </c>
+      <c r="G12" s="1">
+        <v>6.4833220000000003</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0001013476616609</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f>"-xO3 -autopar"</f>
+        <v>-xO3 -autopar</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6.4801460000000004</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6.4800709999999997</v>
+      </c>
+      <c r="G13" s="1">
+        <v>6.4808664</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="2"/>
+        <v>1.000485637206322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f t="shared" ref="A14:A17" si="3">"-xO3 -autopar"</f>
+        <v>-xO3 -autopar</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E14" s="1">
+        <v>6.4798650000000002</v>
+      </c>
+      <c r="F14" s="1">
+        <v>6.4797919999999998</v>
+      </c>
+      <c r="G14" s="1">
+        <v>6.4805609999999998</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="2"/>
+        <v>1.000529023366999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f t="shared" si="3"/>
+        <v>-xO3 -autopar</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E15" s="1">
+        <v>6.4810949999999998</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6.4810179999999997</v>
+      </c>
+      <c r="G15" s="1">
+        <v>6.481776</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0003391402224471</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f t="shared" si="3"/>
+        <v>-xO3 -autopar</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E16" s="1">
+        <v>6.4812599999999998</v>
+      </c>
+      <c r="F16" s="1">
+        <v>6.4811750000000004</v>
+      </c>
+      <c r="G16" s="1">
+        <v>6.4820494000000002</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0003136735758171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f t="shared" si="3"/>
+        <v>-xO3 -autopar</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E17" s="1">
+        <v>6.4835799999999999</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6.4835060000000002</v>
+      </c>
+      <c r="G17" s="1">
+        <v>6.4842871999999998</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.9999557343319585</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
+        <f>"-xO3 -autopar"</f>
+        <v>-xO3 -autopar</v>
+      </c>
+      <c r="B18">
+        <v>32</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E18" s="1">
+        <v>6.4851939999999999</v>
+      </c>
+      <c r="F18" s="1">
+        <v>6.485112</v>
+      </c>
+      <c r="G18" s="1">
+        <v>6.4858975000000001</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.99970687075822251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
+        <f>"-xO3 -autopar -reduction"</f>
+        <v>-xO3 -autopar -reduction</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E19" s="1">
+        <v>6.4561549999999999</v>
+      </c>
+      <c r="F19" s="1">
+        <v>6.4560690000000003</v>
+      </c>
+      <c r="G19" s="1">
+        <v>6.4568715000000001</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0042034306797156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
+        <f t="shared" ref="A20:A24" si="4">"-xO3 -autopar -reduction"</f>
+        <v>-xO3 -autopar -reduction</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3.1415926441379902</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4517997872856085E-9</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3.223061</v>
+      </c>
+      <c r="F20" s="1">
+        <v>6.4450070000000004</v>
+      </c>
+      <c r="G20" s="1">
+        <v>3.2238034999999998</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="2"/>
+        <v>2.0115328254724312</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
+        <f t="shared" si="4"/>
+        <v>-xO3 -autopar -reduction</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3.1415926441370501</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4527399241428611E-9</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1.625418</v>
+      </c>
+      <c r="F21" s="1">
+        <v>6.465859</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1.6261212</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="2"/>
+        <v>3.9886927547252458</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="str">
+        <f t="shared" si="4"/>
+        <v>-xO3 -autopar -reduction</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3.1415926441373601</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4524299498743858E-9</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.11104</v>
+      </c>
+      <c r="F22" s="1">
+        <v>7.4557200000000003</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1.1117359</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="2"/>
+        <v>5.8353371615783409</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="str">
+        <f t="shared" si="4"/>
+        <v>-xO3 -autopar -reduction</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3.14159264413746</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4523300298021695E-9</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.79527999999999999</v>
+      </c>
+      <c r="F23" s="1">
+        <v>12.309901999999999</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.79604830000000004</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="2"/>
+        <v>8.1522143144552857</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f t="shared" si="4"/>
+        <v>-xO3 -autopar -reduction</v>
+      </c>
+      <c r="B24">
+        <v>32</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3.14159264413746</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4523300298021695E-9</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.769957</v>
+      </c>
+      <c r="F24" s="1">
+        <v>24.364322999999999</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.77064440000000001</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="2"/>
+        <v>8.4203312652524751</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f>"-xO3 -xopenmp"</f>
+        <v>-xO3 -xopenmp</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3.14159264413487</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4549199580740151E-9</v>
+      </c>
+      <c r="E25" s="1">
+        <v>6.4835010000000004</v>
+      </c>
+      <c r="F25" s="1">
+        <v>6.4834269999999998</v>
+      </c>
+      <c r="G25" s="1">
+        <v>6.4842003999999998</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="2"/>
+        <v>0.99996791856745293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f t="shared" ref="A26:A30" si="5">"-xO3 -xopenmp"</f>
+        <v>-xO3 -xopenmp</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3.1415926441379902</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4517997872856085E-9</v>
+      </c>
+      <c r="E26" s="1">
+        <v>3.2412999999999998</v>
+      </c>
+      <c r="F26" s="1">
+        <v>6.4812770000000004</v>
+      </c>
+      <c r="G26" s="1">
+        <v>3.2419736000000001</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="2"/>
+        <v>2.0002138031036929</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="str">
+        <f t="shared" si="5"/>
+        <v>-xO3 -xopenmp</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3.1415926441370501</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4527399241428611E-9</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1.641645</v>
+      </c>
+      <c r="F27" s="1">
+        <v>6.5242740000000001</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1.6423186000000001</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="2"/>
+        <v>3.949266132446418</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="str">
+        <f t="shared" si="5"/>
+        <v>-xO3 -xopenmp</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3.1415926441373601</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4524299498743858E-9</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1.126309</v>
+      </c>
+      <c r="F28" s="1">
+        <v>7.5468869999999999</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1.1270058999999999</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="2"/>
+        <v>5.7562294183922882</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="str">
+        <f t="shared" si="5"/>
+        <v>-xO3 -xopenmp</v>
+      </c>
+      <c r="B29">
+        <v>16</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3.14159264413746</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4523300298021695E-9</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.80215999999999998</v>
+      </c>
+      <c r="F29" s="1">
+        <v>12.062481</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.80284833</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="2"/>
+        <v>8.0822940560486689</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="str">
+        <f t="shared" si="5"/>
+        <v>-xO3 -xopenmp</v>
+      </c>
+      <c r="B30">
+        <v>32</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3.14159264413746</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4523300298021695E-9</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.757274</v>
+      </c>
+      <c r="F30" s="1">
+        <v>23.953264000000001</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.75795449999999998</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="2"/>
+        <v>8.5613569196882491</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="19" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14" style="1" customWidth="1"/>
+    <col min="6" max="8" width="10.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3.14159265358979</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f t="shared" ref="A7:A23" si="0">"-xO3"</f>
-        <v>-xO3</v>
+        <f>"-O3"</f>
+        <v>-O3</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>3.14159264413487</v>
+        <v>3.14159259601165</v>
       </c>
       <c r="D7" s="2">
-        <f>ABS($B$3-C7)</f>
-        <v>9.4549199580740151E-9</v>
+        <f>ABS($B$4-C7)</f>
+        <v>5.7578140033598402E-8</v>
       </c>
       <c r="E7" s="1">
-        <v>6.483314</v>
+        <v>3.66</v>
       </c>
       <c r="F7" s="1">
-        <v>6.4832450000000001</v>
+        <v>3.6539999999999999</v>
       </c>
       <c r="G7" s="1">
-        <v>6.4840115999999997</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" ref="H7:H29" si="1">$E$6/E7</f>
-        <v>0.99999676091579082</v>
-      </c>
+        <f>$E$7/E7</f>
+        <v>1</v>
+      </c>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f t="shared" si="0"/>
-        <v>-xO3</v>
+        <f>"-O3 -fopenmp"</f>
+        <v>-O3 -fopenmp</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2">
-        <v>3.14159264413487</v>
+        <v>3.14159259601165</v>
       </c>
       <c r="D8" s="2">
-        <f>ABS($B$3-C8)</f>
-        <v>9.4549199580740151E-9</v>
+        <f>ABS($B$4-C8)</f>
+        <v>5.7578140033598402E-8</v>
       </c>
       <c r="E8" s="1">
-        <v>6.4811430000000003</v>
+        <v>3.702</v>
       </c>
       <c r="F8" s="1">
-        <v>6.4810720000000002</v>
+        <v>3.6909999999999998</v>
       </c>
       <c r="G8" s="1">
-        <v>6.4818515000000003</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0003317316096867</v>
+        <f>$E$7/E8</f>
+        <v>0.9886547811993518</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f t="shared" si="0"/>
-        <v>-xO3</v>
+        <f>"-O3 -fopenmp"</f>
+        <v>-O3 -fopenmp</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2">
-        <v>3.14159264413487</v>
+        <v>3.1415925960281701</v>
       </c>
       <c r="D9" s="2">
-        <f>ABS($B$3-C9)</f>
-        <v>9.4549199580740151E-9</v>
+        <f>ABS($B$4-C9)</f>
+        <v>5.7561619914991979E-8</v>
       </c>
       <c r="E9" s="1">
-        <v>6.4839989999999998</v>
+        <v>1.8640000000000001</v>
       </c>
       <c r="F9" s="1">
-        <v>6.4839260000000003</v>
+        <v>3.7069999999999999</v>
       </c>
       <c r="G9" s="1">
-        <v>6.4846754000000004</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="1"/>
-        <v>0.99989111657790197</v>
+        <f>$E$7/E9</f>
+        <v>1.9635193133047211</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f t="shared" si="0"/>
-        <v>-xO3</v>
+        <f>"-O3 -fopenmp"</f>
+        <v>-O3 -fopenmp</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2">
-        <v>3.14159264413487</v>
+        <v>3.1415925960275999</v>
       </c>
       <c r="D10" s="2">
-        <f>ABS($B$3-C10)</f>
-        <v>9.4549199580740151E-9</v>
+        <f>ABS($B$4-C10)</f>
+        <v>5.7562190125537427E-8</v>
       </c>
       <c r="E10" s="1">
-        <v>6.4901900000000001</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="F10" s="1">
-        <v>6.4901090000000003</v>
+        <v>3.903</v>
       </c>
       <c r="G10" s="1">
-        <v>6.4908904999999999</v>
+        <v>0.01</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="1"/>
-        <v>0.99893731924643181</v>
+        <f>$E$7/E10</f>
+        <v>3.7119675456389456</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f t="shared" si="0"/>
-        <v>-xO3</v>
+        <f>"-O3 -fopenmp"</f>
+        <v>-O3 -fopenmp</v>
       </c>
       <c r="B11">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2">
-        <v>3.14159264413487</v>
+        <v>3.1415925960267899</v>
       </c>
       <c r="D11" s="2">
-        <f>ABS($B$3-C11)</f>
-        <v>9.4549199580740151E-9</v>
+        <f>ABS($B$4-C11)</f>
+        <v>5.7563000144256193E-8</v>
       </c>
       <c r="E11" s="1">
-        <v>6.4826360000000003</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="F11" s="1">
-        <v>6.4825660000000003</v>
+        <v>7.31</v>
       </c>
       <c r="G11" s="1">
-        <v>6.4833220000000003</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0001013476616609</v>
+        <f>$E$7/E11</f>
+        <v>3.8085327783558798</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f>"-xO3 -autopar"</f>
-        <v>-xO3 -autopar</v>
+        <f>"-O3 -fopenmp"</f>
+        <v>-O3 -fopenmp</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2">
-        <v>3.14159264413487</v>
+        <v>3.1415925960269999</v>
       </c>
       <c r="D12" s="2">
-        <f>ABS($B$3-C12)</f>
-        <v>9.4549199580740151E-9</v>
+        <f>ABS($B$4-C12)</f>
+        <v>5.7562790090059934E-8</v>
       </c>
       <c r="E12" s="1">
-        <v>6.4801460000000004</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="F12" s="1">
-        <v>6.4800709999999997</v>
+        <v>7.3579999999999997</v>
       </c>
       <c r="G12" s="1">
-        <v>6.4808664</v>
+        <v>1.9E-2</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="1"/>
-        <v>1.000485637206322</v>
+        <f>$E$7/E12</f>
+        <v>3.8085327783558798</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <f t="shared" ref="A13:A17" si="2">"-xO3 -autopar"</f>
-        <v>-xO3 -autopar</v>
+        <f>"-O3 -fopenmp"</f>
+        <v>-O3 -fopenmp</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2">
-        <v>3.14159264413487</v>
+        <v>3.1415925960267002</v>
       </c>
       <c r="D13" s="2">
-        <f>ABS($B$3-C13)</f>
-        <v>9.4549199580740151E-9</v>
+        <f>ABS($B$4-C13)</f>
+        <v>5.7563089850276583E-8</v>
       </c>
       <c r="E13" s="1">
-        <v>6.4798650000000002</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="F13" s="1">
-        <v>6.4797919999999998</v>
+        <v>7.3780000000000001</v>
       </c>
       <c r="G13" s="1">
-        <v>6.4805609999999998</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="1"/>
-        <v>1.000529023366999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="str">
-        <f t="shared" si="2"/>
-        <v>-xO3 -autopar</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2">
-        <v>3.14159264413487</v>
-      </c>
-      <c r="D14" s="2">
-        <f>ABS($B$3-C14)</f>
-        <v>9.4549199580740151E-9</v>
-      </c>
-      <c r="E14" s="1">
-        <v>6.4810949999999998</v>
-      </c>
-      <c r="F14" s="1">
-        <v>6.4810179999999997</v>
-      </c>
-      <c r="G14" s="1">
-        <v>6.481776</v>
-      </c>
-      <c r="H14" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0003391402224471</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="str">
-        <f t="shared" si="2"/>
-        <v>-xO3 -autopar</v>
-      </c>
-      <c r="B15">
-        <v>8</v>
-      </c>
-      <c r="C15" s="2">
-        <v>3.14159264413487</v>
-      </c>
-      <c r="D15" s="2">
-        <f>ABS($B$3-C15)</f>
-        <v>9.4549199580740151E-9</v>
-      </c>
-      <c r="E15" s="1">
-        <v>6.4812599999999998</v>
-      </c>
-      <c r="F15" s="1">
-        <v>6.4811750000000004</v>
-      </c>
-      <c r="G15" s="1">
-        <v>6.4820494000000002</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0003136735758171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" t="str">
-        <f t="shared" si="2"/>
-        <v>-xO3 -autopar</v>
-      </c>
-      <c r="B16">
-        <v>16</v>
-      </c>
-      <c r="C16" s="2">
-        <v>3.14159264413487</v>
-      </c>
-      <c r="D16" s="2">
-        <f>ABS($B$3-C16)</f>
-        <v>9.4549199580740151E-9</v>
-      </c>
-      <c r="E16" s="1">
-        <v>6.4835799999999999</v>
-      </c>
-      <c r="F16" s="1">
-        <v>6.4835060000000002</v>
-      </c>
-      <c r="G16" s="1">
-        <v>6.4842871999999998</v>
-      </c>
-      <c r="H16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.9999557343319585</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="str">
-        <f>"-xO3 -autopar"</f>
-        <v>-xO3 -autopar</v>
-      </c>
-      <c r="B17">
-        <v>32</v>
-      </c>
-      <c r="C17" s="2">
-        <v>3.14159264413487</v>
-      </c>
-      <c r="D17" s="2">
-        <f>ABS($B$3-C17)</f>
-        <v>9.4549199580740151E-9</v>
-      </c>
-      <c r="E17" s="1">
-        <v>6.4851939999999999</v>
-      </c>
-      <c r="F17" s="1">
-        <v>6.485112</v>
-      </c>
-      <c r="G17" s="1">
-        <v>6.4858975000000001</v>
-      </c>
-      <c r="H17" s="1">
-        <f t="shared" si="1"/>
-        <v>0.99970687075822251</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="str">
-        <f>"-xO3 -autopar -reduction"</f>
-        <v>-xO3 -autopar -reduction</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2">
-        <v>3.14159264413487</v>
-      </c>
-      <c r="D18" s="2">
-        <f>ABS($B$3-C18)</f>
-        <v>9.4549199580740151E-9</v>
-      </c>
-      <c r="E18" s="1">
-        <v>6.4561549999999999</v>
-      </c>
-      <c r="F18" s="1">
-        <v>6.4560690000000003</v>
-      </c>
-      <c r="G18" s="1">
-        <v>6.4568715000000001</v>
-      </c>
-      <c r="H18" s="1">
-        <f t="shared" si="1"/>
-        <v>1.0042034306797156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="str">
-        <f t="shared" ref="A19:A23" si="3">"-xO3 -autopar -reduction"</f>
-        <v>-xO3 -autopar -reduction</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2">
-        <v>3.1415926441379902</v>
-      </c>
-      <c r="D19" s="2">
-        <f>ABS($B$3-C19)</f>
-        <v>9.4517997872856085E-9</v>
-      </c>
-      <c r="E19" s="1">
-        <v>3.223061</v>
-      </c>
-      <c r="F19" s="1">
-        <v>6.4450070000000004</v>
-      </c>
-      <c r="G19" s="1">
-        <v>3.2238034999999998</v>
-      </c>
-      <c r="H19" s="1">
-        <f t="shared" si="1"/>
-        <v>2.0115328254724312</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="str">
-        <f t="shared" si="3"/>
-        <v>-xO3 -autopar -reduction</v>
-      </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20" s="2">
-        <v>3.1415926441370501</v>
-      </c>
-      <c r="D20" s="2">
-        <f>ABS($B$3-C20)</f>
-        <v>9.4527399241428611E-9</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1.625418</v>
-      </c>
-      <c r="F20" s="1">
-        <v>6.465859</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1.6261212</v>
-      </c>
-      <c r="H20" s="1">
-        <f t="shared" si="1"/>
-        <v>3.9886927547252458</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="str">
-        <f t="shared" si="3"/>
-        <v>-xO3 -autopar -reduction</v>
-      </c>
-      <c r="B21">
-        <v>8</v>
-      </c>
-      <c r="C21" s="2">
-        <v>3.1415926441373601</v>
-      </c>
-      <c r="D21" s="2">
-        <f>ABS($B$3-C21)</f>
-        <v>9.4524299498743858E-9</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1.11104</v>
-      </c>
-      <c r="F21" s="1">
-        <v>7.4557200000000003</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1.1117359</v>
-      </c>
-      <c r="H21" s="1">
-        <f t="shared" si="1"/>
-        <v>5.8353371615783409</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="str">
-        <f t="shared" si="3"/>
-        <v>-xO3 -autopar -reduction</v>
-      </c>
-      <c r="B22">
-        <v>16</v>
-      </c>
-      <c r="C22" s="2">
-        <v>3.14159264413746</v>
-      </c>
-      <c r="D22" s="2">
-        <f>ABS($B$3-C22)</f>
-        <v>9.4523300298021695E-9</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.79527999999999999</v>
-      </c>
-      <c r="F22" s="1">
-        <v>12.309901999999999</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0.79604830000000004</v>
-      </c>
-      <c r="H22" s="1">
-        <f t="shared" si="1"/>
-        <v>8.1522143144552857</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="str">
-        <f t="shared" si="3"/>
-        <v>-xO3 -autopar -reduction</v>
-      </c>
-      <c r="B23">
-        <v>32</v>
-      </c>
-      <c r="C23" s="2">
-        <v>3.14159264413746</v>
-      </c>
-      <c r="D23" s="2">
-        <f>ABS($B$3-C23)</f>
-        <v>9.4523300298021695E-9</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.769957</v>
-      </c>
-      <c r="F23" s="1">
-        <v>24.364322999999999</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0.77064440000000001</v>
-      </c>
-      <c r="H23" s="1">
-        <f t="shared" si="1"/>
-        <v>8.4203312652524751</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="str">
-        <f>"-xO3 -xopenmp"</f>
-        <v>-xO3 -xopenmp</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2">
-        <v>3.14159264413487</v>
-      </c>
-      <c r="D24" s="2">
-        <f>ABS($B$3-C24)</f>
-        <v>9.4549199580740151E-9</v>
-      </c>
-      <c r="E24" s="1">
-        <v>6.4835010000000004</v>
-      </c>
-      <c r="F24" s="1">
-        <v>6.4834269999999998</v>
-      </c>
-      <c r="G24" s="1">
-        <v>6.4842003999999998</v>
-      </c>
-      <c r="H24" s="1">
-        <f t="shared" si="1"/>
-        <v>0.99996791856745293</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="str">
-        <f t="shared" ref="A25:A29" si="4">"-xO3 -xopenmp"</f>
-        <v>-xO3 -xopenmp</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25" s="2">
-        <v>3.1415926441379902</v>
-      </c>
-      <c r="D25" s="2">
-        <f>ABS($B$3-C25)</f>
-        <v>9.4517997872856085E-9</v>
-      </c>
-      <c r="E25" s="1">
-        <v>3.2412999999999998</v>
-      </c>
-      <c r="F25" s="1">
-        <v>6.4812770000000004</v>
-      </c>
-      <c r="G25" s="1">
-        <v>3.2419736000000001</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" si="1"/>
-        <v>2.0002138031036929</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="str">
-        <f t="shared" si="4"/>
-        <v>-xO3 -xopenmp</v>
-      </c>
-      <c r="B26">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2">
-        <v>3.1415926441370501</v>
-      </c>
-      <c r="D26" s="2">
-        <f>ABS($B$3-C26)</f>
-        <v>9.4527399241428611E-9</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1.641645</v>
-      </c>
-      <c r="F26" s="1">
-        <v>6.5242740000000001</v>
-      </c>
-      <c r="G26" s="1">
-        <v>1.6423186000000001</v>
-      </c>
-      <c r="H26" s="1">
-        <f t="shared" si="1"/>
-        <v>3.949266132446418</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="str">
-        <f t="shared" si="4"/>
-        <v>-xO3 -xopenmp</v>
-      </c>
-      <c r="B27">
-        <v>8</v>
-      </c>
-      <c r="C27" s="2">
-        <v>3.1415926441373601</v>
-      </c>
-      <c r="D27" s="2">
-        <f>ABS($B$3-C27)</f>
-        <v>9.4524299498743858E-9</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1.126309</v>
-      </c>
-      <c r="F27" s="1">
-        <v>7.5468869999999999</v>
-      </c>
-      <c r="G27" s="1">
-        <v>1.1270058999999999</v>
-      </c>
-      <c r="H27" s="1">
-        <f t="shared" si="1"/>
-        <v>5.7562294183922882</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="str">
-        <f t="shared" si="4"/>
-        <v>-xO3 -xopenmp</v>
-      </c>
-      <c r="B28">
-        <v>16</v>
-      </c>
-      <c r="C28" s="2">
-        <v>3.14159264413746</v>
-      </c>
-      <c r="D28" s="2">
-        <f>ABS($B$3-C28)</f>
-        <v>9.4523300298021695E-9</v>
-      </c>
-      <c r="E28" s="1">
-        <v>0.80215999999999998</v>
-      </c>
-      <c r="F28" s="1">
-        <v>12.062481</v>
-      </c>
-      <c r="G28" s="1">
-        <v>0.80284833</v>
-      </c>
-      <c r="H28" s="1">
-        <f t="shared" si="1"/>
-        <v>8.0822940560486689</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="str">
-        <f t="shared" si="4"/>
-        <v>-xO3 -xopenmp</v>
-      </c>
-      <c r="B29">
-        <v>32</v>
-      </c>
-      <c r="C29" s="2">
-        <v>3.14159264413746</v>
-      </c>
-      <c r="D29" s="2">
-        <f>ABS($B$3-C29)</f>
-        <v>9.4523300298021695E-9</v>
-      </c>
-      <c r="E29" s="1">
-        <v>0.757274</v>
-      </c>
-      <c r="F29" s="1">
-        <v>23.953264000000001</v>
-      </c>
-      <c r="G29" s="1">
-        <v>0.75795449999999998</v>
-      </c>
-      <c r="H29" s="1">
-        <f t="shared" si="1"/>
-        <v>8.5613569196882491</v>
+        <f>$E$7/E13</f>
+        <v>3.8085327783558798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>